<commit_message>
change to default epochs
</commit_message>
<xml_diff>
--- a/examples/experiment1/data_odenet_False.xlsx
+++ b/examples/experiment1/data_odenet_False.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="batch_size_64" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="batch_size_1.0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3007354736328125</v>
+        <v>0.5070674419403076</v>
       </c>
       <c r="C2" t="n">
         <v>32</v>
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0902</v>
+        <v>0.1021833333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0891</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3793339729309082</v>
+        <v>0.5948929786682129</v>
       </c>
       <c r="C3" t="n">
-        <v>20.00287763947754</v>
+        <v>20.28106538184927</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9807166666666667</v>
+        <v>0.9706166666666667</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9816</v>
+        <v>0.9752999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>